<commit_message>
Ditto Pachen- Merge from Branch May 14
</commit_message>
<xml_diff>
--- a/SSAS/Development/Artifacts/Changes From 05 May.xlsx
+++ b/SSAS/Development/Artifacts/Changes From 05 May.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>Bugzilla Ticket No</t>
   </si>
@@ -204,7 +204,22 @@
 </t>
   </si>
   <si>
-    <t>Import the workflow from admin and release the process.</t>
+    <t>Import the intake script from the admin.</t>
+  </si>
+  <si>
+    <t>Import the workflow from admin and release the process.
+Or 
+importworkflows -Dworkflow.dir=  -Doverwrite=true</t>
+  </si>
+  <si>
+    <t>Import using the admin</t>
+  </si>
+  <si>
+    <t>INSERT INTO WORKQUEUE (ADMINISTRATORUSERNAME, ALLOWUSERSUBSCRIPTIONIND, COMMENTS, LASTWRITTEN, NAME, SENSITIVITY, UPPERNAME, VERSIONNO, WORKQUEUEID) VALUES ('admin', '1', 'This work queue is used to assign tasks to case workers when the applications have exceeded 90 days.', '2001-01-01 00:00:00', 'Application Follow-up: Applications that have exceeded 90 days', '1', 'APPLICATION FOLLOW-UP: APPLICATIONS THAT HAVE EXCEEDED 90 DAYS', 1, 45012);
+INSERT INTO ALLOCATIONTARGETITEM (ALLOCATIONTARGETID, ALLOCATIONTARGETITEMID, RELATEDID, RELATEDNAME, TYPE) VALUES ('ApplicationFollowUp', 45005, 45012, 'ApplicationFollowUp', 'RL23');
+INSERT INTO ALLOCATIONTARGET (ALLOCATIONTARGETID, COMMENTS, NAME) VALUES ('ApplicationFollowUp', 'Application follow up work queue for the case worker.', 'ApplicationFollowUp');
+update milestoneconfiguration set duration=90 where milestoneConfigurationID=45001;
+INSERT INTO WORKQUEUE (ADMINISTRATORUSERNAME, ALLOWUSERSUBSCRIPTIONIND, COMMENTS, LASTWRITTEN, NAME, SENSITIVITY, UPPERNAME, VERSIONNO, WORKQUEUEID) VALUES ('admin', '1', 'This work queue is used to assign tasks to case workers when the applications have exceeded 90 days.', '2001-01-01 00:00:00', 'متابعة الطلب : الطلبات التي تجاوزت 90 يوما', '1', 'APPLICATION FOLLOW-UP: APPLICATIONS THAT HAVE EXCEEDED 90 DAYS', 1, 45012);</t>
   </si>
 </sst>
 </file>
@@ -594,9 +609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +699,9 @@
         <v>16</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -752,6 +769,12 @@
       <c r="F9" t="s">
         <v>16</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -766,8 +789,8 @@
       <c r="F10" t="s">
         <v>16</v>
       </c>
-      <c r="I10" t="s">
-        <v>28</v>
+      <c r="I10" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -782,65 +805,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
+      <Description>UQKZYU5EZKJQ-17-950</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003520CC91E1C90A4F9689A135D663C63F" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5bea9beecb72e899f05172e22af69af0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e967487d-3eea-483d-b969-e50e6c114ffa" xmlns:ns3="43475cab-d89f-451e-a1e3-4db005e0f558" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="438d5435a0413bb8242127eebe6f163c" ns2:_="" ns3:_="">
     <xsd:import namespace="e967487d-3eea-483d-b969-e50e6c114ffa"/>
@@ -1024,42 +1007,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=15.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">UQKZYU5EZKJQ-17-950</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <Url>https://dionatec.sharepoint.com/GlobalServices/_layouts/15/DocIdRedir.aspx?ID=UQKZYU5EZKJQ-17-950</Url>
-      <Description>UQKZYU5EZKJQ-17-950</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="e967487d-3eea-483d-b969-e50e6c114ffa">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
+    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0051AA5-43D6-41A0-9086-D5D3DFF72221}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1078,19 +1102,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6F0B25-6AD0-4AF9-AE4F-0D8285608470}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1926F8BC-3749-487B-86BA-515B8CAD861D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A3CD956-F256-4860-8B56-AE881D5ADEC8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="e967487d-3eea-483d-b969-e50e6c114ffa"/>
-    <ds:schemaRef ds:uri="43475cab-d89f-451e-a1e3-4db005e0f558"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>